<commit_message>
Updated Backlog, Added Sprint Backlog
Backlog is now up to date with user stories. Kanban matches. Sprint 1 Backlog now exists and matches User stories and Product Backlog, Need to establish Product Backlog priority and story points.
</commit_message>
<xml_diff>
--- a/Product_Backlog_RootDigital.xlsx
+++ b/Product_Backlog_RootDigital.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\Root-Digital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F19390-CE9D-4734-916D-C962699D078A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F02737-9D8E-4BC2-8300-DE40E02A2625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="2115" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>User Story</t>
   </si>
@@ -44,30 +44,10 @@
     so I can multitask while using the application</t>
   </si>
   <si>
-    <t>As a user, I want the alarm to vibrate/make a noise,   
-    so I know when to switch activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> As a developer, I want to receive reports/bugs from users,
-    so I can fix them quickly and efficently.</t>
-  </si>
-  <si>
-    <t>As a user, I want to opt into and out of notifications to use the app
-    so I can be reminded to use the application.</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to donate to the developers, 
     so I can reward them for creating a helpful application.</t>
   </si>
   <si>
-    <t>As a user, I want to choose different Pomodoro intervals
-	so I can manage my time how I want.</t>
-  </si>
-  <si>
-    <t>As a user, I want to choose different alarms/ringtones
-	so I can personilize it for me.</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to schedule my day,
 	so I spend my time wisely.</t>
   </si>
@@ -76,10 +56,6 @@
 	so I can make it more appealing.</t>
   </si>
   <si>
-    <t>As a user, I want some motivational quotes/media,
-	so I can motivate myself.</t>
-  </si>
-  <si>
     <t>As a fitness coach, I want to share custom workouts,
 	so that I can have my trainee follow it when I'm not there.</t>
   </si>
@@ -100,10 +76,6 @@
 	so that me and my partner can go through this experience together.</t>
   </si>
   <si>
-    <t>As a college student, I want to have access to exercises I can do in my chair,
-	so that I can I can use this app in the library.</t>
-  </si>
-  <si>
     <t>As a desk-job-worker, I want stretches to be included as available exercises,
 	so that I can keep my back, neck, and shoulders healthy during long days.</t>
   </si>
@@ -112,12 +84,55 @@
 	so that I can manage my stress while remaining productive.</t>
   </si>
   <si>
-    <t>As a novice to fitness, I want visuals to help guide me during exercises,
-	so that I can use the app without having to stop to research forms.</t>
-  </si>
-  <si>
-    <t>As a novice to fitness, I want allow the app to randomly select exercises for me,
-	so that I can see which ones work best for me.</t>
+    <t>As a user, I want the alarm to vibrate,   
+    so I know when to switch activities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want the alarm to make a noise,
+	So I know when to switch activities.  </t>
+  </si>
+  <si>
+    <t>As a user, I want to send feedback to the developers,
+    so they know how I feel about their app.</t>
+  </si>
+  <si>
+    <t>As a user, I want to report bugs I find, 
+	so they can be fixed quickly and efficiently.</t>
+  </si>
+  <si>
+    <t>As a user, I want to opt into and out of notifications to use the app,
+    so I can be reminded to use the application.</t>
+  </si>
+  <si>
+    <t>As a user, I want to choose different Pomodoro intervals,
+so I can manage my time how I want.</t>
+  </si>
+  <si>
+    <t>As a user, I want to choose different alarms,
+so I can personilize it for me.</t>
+  </si>
+  <si>
+    <t>As a user, I want some motivational quotes,
+	so I can motivate myself.</t>
+  </si>
+  <si>
+    <t>As a user, I want some motivational media, 
+	so I can motivate myself.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a college student, I want to have access to exercises I can do in my chair,
+	so that I can I can use this app in the library. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a novice to fitness, I want visuals to help guide me during exercises,
+	so that I can use the app without having to stop to research forms. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a novice to fitness, I want allow the app to randomly select exercises for me,
+	so that I can see which ones work best for me. </t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -423,8 +438,8 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B23:B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -471,31 +486,43 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -507,7 +534,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -519,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -531,7 +558,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -543,19 +570,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="1"/>
@@ -567,7 +600,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -579,7 +612,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -591,7 +624,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="1"/>
@@ -603,7 +636,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -615,7 +648,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -627,7 +660,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -639,7 +672,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -651,7 +684,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -663,7 +696,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -675,7 +708,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -687,36 +720,44 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="5"/>
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>

</xml_diff>

<commit_message>
File Names and Proj Backlog
File names match required naming convention.  Project Backlog now has estimates of points and sprints for each story.
</commit_message>
<xml_diff>
--- a/Product_Backlog_RootDigital.xlsx
+++ b/Product_Backlog_RootDigital.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\Root-Digital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F02737-9D8E-4BC2-8300-DE40E02A2625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B00AD4-02B7-4F94-8B05-5B8B514169E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="2115" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6690" yWindow="3015" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>User Story</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Urgent</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -438,14 +453,14 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="111.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="59" style="7" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -476,10 +491,18 @@
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -491,7 +514,9 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
@@ -509,7 +534,9 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>29</v>
       </c>
@@ -524,10 +551,18 @@
       <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -536,22 +571,38 @@
       <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -560,10 +611,18 @@
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="3"/>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -575,12 +634,14 @@
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -591,9 +652,15 @@
         <v>8</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="3"/>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -602,10 +669,18 @@
       <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3"/>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -614,10 +689,18 @@
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="3"/>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -626,10 +709,18 @@
       <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="3"/>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -638,10 +729,18 @@
       <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -650,22 +749,38 @@
       <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="3"/>
+      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -674,94 +789,158 @@
       <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>

</xml_diff>